<commit_message>
Added factor to example dataset files
</commit_message>
<xml_diff>
--- a/example/Default_QC.xlsx
+++ b/example/Default_QC.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="137">
   <si>
     <t>Custom Segment Name</t>
   </si>
@@ -83,15 +83,18 @@
     <t>ROI_ID</t>
   </si>
   <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
     <t>Scan_ID_1</t>
   </si>
   <si>
     <t>ROI_ID_1</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>AOI_size</t>
   </si>
   <si>
@@ -266,9 +269,6 @@
     <t>PanCK</t>
   </si>
   <si>
-    <t>PanCK,PanCK</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -281,6 +281,9 @@
     <t>200</t>
   </si>
   <si>
+    <t>Tumour</t>
+  </si>
+  <si>
     <t>Protein Training Scan 2 | 001 | PanCK-</t>
   </si>
   <si>
@@ -290,7 +293,7 @@
     <t>PanCK-</t>
   </si>
   <si>
-    <t>PanCK-,PanCK-</t>
+    <t>TME</t>
   </si>
   <si>
     <t>Protein Training Scan 2 | 002 | PanCK</t>
@@ -502,49 +505,49 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="R1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
@@ -552,49 +555,49 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="P2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="R2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="S2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3">
@@ -602,49 +605,49 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="P3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
@@ -652,49 +655,49 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="M4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="S4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5">
@@ -702,49 +705,49 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
@@ -1418,158 +1421,158 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="P21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="R21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="K22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="L22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="M22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="N22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="P22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="R22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="S22" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="J23" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="K23" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="L23" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="M23" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="N23" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="O23" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="P23" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="Q23" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="R23" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="S23" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24">
@@ -1577,52 +1580,52 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="K24" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="L24" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="M24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N24" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O24" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P24" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="Q24" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="R24" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="S24" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25">
@@ -1630,1428 +1633,1481 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" t="s">
+        <v>118</v>
+      </c>
+      <c r="N25" t="s">
+        <v>118</v>
+      </c>
+      <c r="O25" t="s">
+        <v>118</v>
+      </c>
+      <c r="P25" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>118</v>
+      </c>
+      <c r="R25" t="s">
+        <v>118</v>
+      </c>
+      <c r="S25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" t="n">
-        <v>1077.7935169563407</v>
-      </c>
-      <c r="F26" t="n">
-        <v>4641.436122323263</v>
-      </c>
-      <c r="G26" t="n">
-        <v>144.2486356153046</v>
-      </c>
-      <c r="H26" t="n">
-        <v>440.5457994425575</v>
-      </c>
-      <c r="I26" t="n">
-        <v>4079.717242512663</v>
-      </c>
-      <c r="J26" t="n">
-        <v>158.0825828450218</v>
-      </c>
-      <c r="K26" t="n">
-        <v>21348.14340816034</v>
-      </c>
-      <c r="L26" t="n">
-        <v>5541.761484533707</v>
-      </c>
-      <c r="M26" t="n">
-        <v>1727.704485797263</v>
-      </c>
-      <c r="N26" t="n">
-        <v>32789.350577392324</v>
-      </c>
-      <c r="O26" t="n">
-        <v>73506.6687874044</v>
-      </c>
-      <c r="P26" t="n">
-        <v>8269.40763212902</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>49891.52340401718</v>
-      </c>
-      <c r="R26" t="n">
-        <v>18275.216069677692</v>
-      </c>
-      <c r="S26" t="n">
-        <v>93435.62043197716</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E27" t="n">
-        <v>54.14953033684346</v>
+        <v>1077.7935169563407</v>
       </c>
       <c r="F27" t="n">
         <v>4641.436122323263</v>
       </c>
       <c r="G27" t="n">
-        <v>4.9669660343130095</v>
+        <v>144.2486356153046</v>
       </c>
       <c r="H27" t="n">
-        <v>22.64282065078084</v>
+        <v>440.5457994425575</v>
       </c>
       <c r="I27" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J27" t="n">
-        <v>5.544629222545217</v>
+        <v>158.0825828450218</v>
       </c>
       <c r="K27" t="n">
-        <v>163.4622216122922</v>
+        <v>21348.14340816034</v>
       </c>
       <c r="L27" t="n">
-        <v>38.2687749759657</v>
+        <v>5541.761484533707</v>
       </c>
       <c r="M27" t="n">
-        <v>15.720650983358242</v>
+        <v>1727.704485797263</v>
       </c>
       <c r="N27" t="n">
-        <v>894.3105769274697</v>
+        <v>32789.350577392324</v>
       </c>
       <c r="O27" t="n">
-        <v>421.08101818725305</v>
+        <v>73506.6687874044</v>
       </c>
       <c r="P27" t="n">
-        <v>110.61476267167798</v>
+        <v>8269.40763212902</v>
       </c>
       <c r="Q27" t="n">
-        <v>322.7388628296871</v>
+        <v>49891.52340401718</v>
       </c>
       <c r="R27" t="n">
-        <v>433.2161428016602</v>
+        <v>18275.216069677692</v>
       </c>
       <c r="S27" t="n">
-        <v>486.544766495858</v>
+        <v>93435.62043197716</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E28" t="n">
-        <v>75.22794156239972</v>
+        <v>54.14953033684346</v>
       </c>
       <c r="F28" t="n">
-        <v>46779.747922125905</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G28" t="n">
-        <v>18.465019125176667</v>
+        <v>4.9669660343130095</v>
       </c>
       <c r="H28" t="n">
-        <v>34.660770831718445</v>
+        <v>22.64282065078084</v>
       </c>
       <c r="I28" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J28" t="n">
-        <v>10.392867015211218</v>
+        <v>5.544629222545217</v>
       </c>
       <c r="K28" t="n">
-        <v>269.0192154809943</v>
+        <v>163.4622216122922</v>
       </c>
       <c r="L28" t="n">
-        <v>59.67194893877422</v>
+        <v>38.2687749759657</v>
       </c>
       <c r="M28" t="n">
-        <v>26.356440509352286</v>
+        <v>15.720650983358242</v>
       </c>
       <c r="N28" t="n">
-        <v>300.35757511778496</v>
+        <v>894.3105769274697</v>
       </c>
       <c r="O28" t="n">
-        <v>455.89123760885604</v>
+        <v>421.08101818725305</v>
       </c>
       <c r="P28" t="n">
-        <v>75.72292868963989</v>
+        <v>110.61476267167798</v>
       </c>
       <c r="Q28" t="n">
-        <v>395.2148026518229</v>
+        <v>322.7388628296871</v>
       </c>
       <c r="R28" t="n">
-        <v>164.7745947081262</v>
+        <v>433.2161428016602</v>
       </c>
       <c r="S28" t="n">
-        <v>553.924237863077</v>
+        <v>486.544766495858</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E29" t="n">
-        <v>73178.862264355</v>
+        <v>75.22794156239972</v>
       </c>
       <c r="F29" t="n">
-        <v>4635.238056387356</v>
+        <v>46779.747922125905</v>
       </c>
       <c r="G29" t="n">
-        <v>6616.16731556225</v>
+        <v>18.465019125176667</v>
       </c>
       <c r="H29" t="n">
-        <v>30324.272167690993</v>
+        <v>34.660770831718445</v>
       </c>
       <c r="I29" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J29" t="n">
-        <v>10529.52077415805</v>
+        <v>10.392867015211218</v>
       </c>
       <c r="K29" t="n">
-        <v>213652.2702340764</v>
+        <v>269.0192154809943</v>
       </c>
       <c r="L29" t="n">
-        <v>54382.30864087279</v>
+        <v>59.67194893877422</v>
       </c>
       <c r="M29" t="n">
-        <v>17467.58836146408</v>
+        <v>26.356440509352286</v>
       </c>
       <c r="N29" t="n">
-        <v>4891.795588043898</v>
+        <v>300.35757511778496</v>
       </c>
       <c r="O29" t="n">
-        <v>7302.181415311247</v>
+        <v>455.89123760885604</v>
       </c>
       <c r="P29" t="n">
-        <v>1805.436905279968</v>
+        <v>75.72292868963989</v>
       </c>
       <c r="Q29" t="n">
-        <v>11283.85664618966</v>
+        <v>395.2148026518229</v>
       </c>
       <c r="R29" t="n">
-        <v>2352.1271754100653</v>
+        <v>164.7745947081262</v>
       </c>
       <c r="S29" t="n">
-        <v>6762.073196122759</v>
+        <v>553.924237863077</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E30" t="n">
-        <v>575.9235718330003</v>
+        <v>73178.862264355</v>
       </c>
       <c r="F30" t="n">
-        <v>4313.404017178731</v>
+        <v>4635.238056387356</v>
       </c>
       <c r="G30" t="n">
-        <v>56.08556879642487</v>
+        <v>6616.16731556225</v>
       </c>
       <c r="H30" t="n">
-        <v>270.91853615636325</v>
+        <v>30324.272167690993</v>
       </c>
       <c r="I30" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J30" t="n">
-        <v>81.83809323741606</v>
+        <v>10529.52077415805</v>
       </c>
       <c r="K30" t="n">
-        <v>2180.3145707636822</v>
+        <v>213652.2702340764</v>
       </c>
       <c r="L30" t="n">
-        <v>396.892946083918</v>
+        <v>54382.30864087279</v>
       </c>
       <c r="M30" t="n">
-        <v>158.77562662316825</v>
+        <v>17467.58836146408</v>
       </c>
       <c r="N30" t="n">
-        <v>3755.211432623886</v>
+        <v>4891.795588043898</v>
       </c>
       <c r="O30" t="n">
-        <v>5771.305355328273</v>
+        <v>7302.181415311247</v>
       </c>
       <c r="P30" t="n">
-        <v>795.2386883170483</v>
+        <v>1805.436905279968</v>
       </c>
       <c r="Q30" t="n">
-        <v>3784.696835614711</v>
+        <v>11283.85664618966</v>
       </c>
       <c r="R30" t="n">
-        <v>1885.4482463689167</v>
+        <v>2352.1271754100653</v>
       </c>
       <c r="S30" t="n">
-        <v>6801.731246277091</v>
+        <v>6762.073196122759</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E31" t="n">
-        <v>573.3647505371391</v>
+        <v>575.9235718330003</v>
       </c>
       <c r="F31" t="n">
-        <v>4641.436122323263</v>
+        <v>4313.404017178731</v>
       </c>
       <c r="G31" t="n">
-        <v>42.575240748095354</v>
+        <v>56.08556879642487</v>
       </c>
       <c r="H31" t="n">
-        <v>237.72786482297957</v>
+        <v>270.91853615636325</v>
       </c>
       <c r="I31" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J31" t="n">
-        <v>75.20721932572263</v>
+        <v>81.83809323741606</v>
       </c>
       <c r="K31" t="n">
-        <v>9367.142612233776</v>
+        <v>2180.3145707636822</v>
       </c>
       <c r="L31" t="n">
-        <v>2040.573481246674</v>
+        <v>396.892946083918</v>
       </c>
       <c r="M31" t="n">
-        <v>752.0795291155299</v>
+        <v>158.77562662316825</v>
       </c>
       <c r="N31" t="n">
-        <v>3736.059885801859</v>
+        <v>3755.211432623886</v>
       </c>
       <c r="O31" t="n">
-        <v>6428.394573058066</v>
+        <v>5771.305355328273</v>
       </c>
       <c r="P31" t="n">
-        <v>903.1645269801413</v>
+        <v>795.2386883170483</v>
       </c>
       <c r="Q31" t="n">
-        <v>3989.2286359143227</v>
+        <v>3784.696835614711</v>
       </c>
       <c r="R31" t="n">
-        <v>2552.206993883045</v>
+        <v>1885.4482463689167</v>
       </c>
       <c r="S31" t="n">
-        <v>12820.504183764711</v>
+        <v>6801.731246277091</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E32" t="n">
-        <v>273.45204293375747</v>
+        <v>573.3647505371391</v>
       </c>
       <c r="F32" t="n">
-        <v>9015.557705455658</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G32" t="n">
-        <v>23.445180646824618</v>
+        <v>42.575240748095354</v>
       </c>
       <c r="H32" t="n">
-        <v>117.6698140594943</v>
+        <v>237.72786482297957</v>
       </c>
       <c r="I32" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J32" t="n">
-        <v>37.154720993207405</v>
+        <v>75.20721932572263</v>
       </c>
       <c r="K32" t="n">
-        <v>871.7666462039789</v>
+        <v>9367.142612233776</v>
       </c>
       <c r="L32" t="n">
-        <v>186.03657899030793</v>
+        <v>2040.573481246674</v>
       </c>
       <c r="M32" t="n">
-        <v>73.17433283424343</v>
+        <v>752.0795291155299</v>
       </c>
       <c r="N32" t="n">
-        <v>900.1858894862204</v>
+        <v>3736.059885801859</v>
       </c>
       <c r="O32" t="n">
-        <v>1611.8730803034741</v>
+        <v>6428.394573058066</v>
       </c>
       <c r="P32" t="n">
-        <v>259.11222005849424</v>
+        <v>903.1645269801413</v>
       </c>
       <c r="Q32" t="n">
-        <v>1204.0514502862036</v>
+        <v>3989.2286359143227</v>
       </c>
       <c r="R32" t="n">
-        <v>423.0122324814596</v>
+        <v>2552.206993883045</v>
       </c>
       <c r="S32" t="n">
-        <v>1617.8097821506074</v>
+        <v>12820.504183764711</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E33" t="n">
-        <v>907.9095953773285</v>
+        <v>273.45204293375747</v>
       </c>
       <c r="F33" t="n">
-        <v>5006.079842427382</v>
+        <v>9015.557705455658</v>
       </c>
       <c r="G33" t="n">
-        <v>122.04782215710138</v>
+        <v>23.445180646824618</v>
       </c>
       <c r="H33" t="n">
-        <v>414.28706673219136</v>
+        <v>117.6698140594943</v>
       </c>
       <c r="I33" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J33" t="n">
-        <v>123.78568640466048</v>
+        <v>37.154720993207405</v>
       </c>
       <c r="K33" t="n">
-        <v>2727.118185210819</v>
+        <v>871.7666462039789</v>
       </c>
       <c r="L33" t="n">
-        <v>820.9548571785276</v>
+        <v>186.03657899030793</v>
       </c>
       <c r="M33" t="n">
-        <v>230.05498602739254</v>
+        <v>73.17433283424343</v>
       </c>
       <c r="N33" t="n">
-        <v>1948.2238402008013</v>
+        <v>900.1858894862204</v>
       </c>
       <c r="O33" t="n">
-        <v>3709.600242629768</v>
+        <v>1611.8730803034741</v>
       </c>
       <c r="P33" t="n">
-        <v>544.1939815315175</v>
+        <v>259.11222005849424</v>
       </c>
       <c r="Q33" t="n">
-        <v>2822.211500245826</v>
+        <v>1204.0514502862036</v>
       </c>
       <c r="R33" t="n">
-        <v>979.3410334023489</v>
+        <v>423.0122324814596</v>
       </c>
       <c r="S33" t="n">
-        <v>3944.3673580107943</v>
+        <v>1617.8097821506074</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E34" t="n">
-        <v>2597.2812789648196</v>
+        <v>907.9095953773285</v>
       </c>
       <c r="F34" t="n">
-        <v>4641.436122323263</v>
+        <v>5006.079842427382</v>
       </c>
       <c r="G34" t="n">
-        <v>310.82339384585794</v>
+        <v>122.04782215710138</v>
       </c>
       <c r="H34" t="n">
-        <v>1067.3360310113833</v>
+        <v>414.28706673219136</v>
       </c>
       <c r="I34" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J34" t="n">
-        <v>248.58566707588952</v>
+        <v>123.78568640466048</v>
       </c>
       <c r="K34" t="n">
-        <v>2198.237494995468</v>
+        <v>2727.118185210819</v>
       </c>
       <c r="L34" t="n">
-        <v>467.1702869104895</v>
+        <v>820.9548571785276</v>
       </c>
       <c r="M34" t="n">
-        <v>175.30470837175395</v>
+        <v>230.05498602739254</v>
       </c>
       <c r="N34" t="n">
-        <v>7786.141927523382</v>
+        <v>1948.2238402008013</v>
       </c>
       <c r="O34" t="n">
-        <v>17856.332067961364</v>
+        <v>3709.600242629768</v>
       </c>
       <c r="P34" t="n">
-        <v>1715.893879054053</v>
+        <v>544.1939815315175</v>
       </c>
       <c r="Q34" t="n">
-        <v>10624.964076377399</v>
+        <v>2822.211500245826</v>
       </c>
       <c r="R34" t="n">
-        <v>5259.194066472862</v>
+        <v>979.3410334023489</v>
       </c>
       <c r="S34" t="n">
-        <v>35100.212856868144</v>
+        <v>3944.3673580107943</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E35" t="n">
-        <v>2600.004052927548</v>
+        <v>2597.2812789648196</v>
       </c>
       <c r="F35" t="n">
-        <v>9390.065439801952</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G35" t="n">
-        <v>291.50297361936833</v>
+        <v>310.82339384585794</v>
       </c>
       <c r="H35" t="n">
-        <v>1124.428018069576</v>
+        <v>1067.3360310113833</v>
       </c>
       <c r="I35" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J35" t="n">
-        <v>317.6167614207323</v>
+        <v>248.58566707588952</v>
       </c>
       <c r="K35" t="n">
-        <v>3837.1571457310906</v>
+        <v>2198.237494995468</v>
       </c>
       <c r="L35" t="n">
-        <v>791.929596324721</v>
+        <v>467.1702869104895</v>
       </c>
       <c r="M35" t="n">
-        <v>295.19509571143993</v>
+        <v>175.30470837175395</v>
       </c>
       <c r="N35" t="n">
-        <v>3247.0774028035803</v>
+        <v>7786.141927523382</v>
       </c>
       <c r="O35" t="n">
-        <v>5103.168609193552</v>
+        <v>17856.332067961364</v>
       </c>
       <c r="P35" t="n">
-        <v>836.227018129623</v>
+        <v>1715.893879054053</v>
       </c>
       <c r="Q35" t="n">
-        <v>4367.643482076672</v>
+        <v>10624.964076377399</v>
       </c>
       <c r="R35" t="n">
-        <v>1621.0851795606409</v>
+        <v>5259.194066472862</v>
       </c>
       <c r="S35" t="n">
-        <v>5745.984809431239</v>
+        <v>35100.212856868144</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E36" t="n">
-        <v>69952.08759620192</v>
+        <v>2600.004052927548</v>
       </c>
       <c r="F36" t="n">
-        <v>26186.870482989732</v>
+        <v>9390.065439801952</v>
       </c>
       <c r="G36" t="n">
-        <v>6357.098027891653</v>
+        <v>291.50297361936833</v>
       </c>
       <c r="H36" t="n">
-        <v>30092.81491511839</v>
+        <v>1124.428018069576</v>
       </c>
       <c r="I36" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J36" t="n">
-        <v>8178.357594903368</v>
+        <v>317.6167614207323</v>
       </c>
       <c r="K36" t="n">
-        <v>236300.2154328663</v>
+        <v>3837.1571457310906</v>
       </c>
       <c r="L36" t="n">
-        <v>48626.8157850243</v>
+        <v>791.929596324721</v>
       </c>
       <c r="M36" t="n">
-        <v>18720.67589067789</v>
+        <v>295.19509571143993</v>
       </c>
       <c r="N36" t="n">
-        <v>242716.27955445234</v>
+        <v>3247.0774028035803</v>
       </c>
       <c r="O36" t="n">
-        <v>453531.6992565606</v>
+        <v>5103.168609193552</v>
       </c>
       <c r="P36" t="n">
-        <v>71501.58106164439</v>
+        <v>836.227018129623</v>
       </c>
       <c r="Q36" t="n">
-        <v>354829.6185904965</v>
+        <v>4367.643482076672</v>
       </c>
       <c r="R36" t="n">
-        <v>103175.98566745238</v>
+        <v>1621.0851795606409</v>
       </c>
       <c r="S36" t="n">
-        <v>405422.0477858322</v>
+        <v>5745.984809431239</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E37" t="n">
-        <v>888.5638302784723</v>
+        <v>69952.08759620192</v>
       </c>
       <c r="F37" t="n">
-        <v>4583.319164948736</v>
+        <v>26186.870482989732</v>
       </c>
       <c r="G37" t="n">
-        <v>74.4939673277577</v>
+        <v>6357.098027891653</v>
       </c>
       <c r="H37" t="n">
-        <v>356.312828375576</v>
+        <v>30092.81491511839</v>
       </c>
       <c r="I37" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J37" t="n">
-        <v>100.50200976380124</v>
+        <v>8178.357594903368</v>
       </c>
       <c r="K37" t="n">
-        <v>2708.5809558041733</v>
+        <v>236300.2154328663</v>
       </c>
       <c r="L37" t="n">
-        <v>603.895793016975</v>
+        <v>48626.8157850243</v>
       </c>
       <c r="M37" t="n">
-        <v>202.7677542520418</v>
+        <v>18720.67589067789</v>
       </c>
       <c r="N37" t="n">
-        <v>2780.6461354776684</v>
+        <v>242716.27955445234</v>
       </c>
       <c r="O37" t="n">
-        <v>5037.535685479224</v>
+        <v>453531.6992565606</v>
       </c>
       <c r="P37" t="n">
-        <v>671.8897705561623</v>
+        <v>71501.58106164439</v>
       </c>
       <c r="Q37" t="n">
-        <v>2833.791872132946</v>
+        <v>354829.6185904965</v>
       </c>
       <c r="R37" t="n">
-        <v>1181.174668111491</v>
+        <v>103175.98566745238</v>
       </c>
       <c r="S37" t="n">
-        <v>7349.080815703511</v>
+        <v>405422.0477858322</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="E38" t="n">
-        <v>89.39994231252723</v>
+        <v>888.5638302784723</v>
       </c>
       <c r="F38" t="n">
-        <v>4641.436122323263</v>
+        <v>4583.319164948736</v>
       </c>
       <c r="G38" t="n">
-        <v>10.775372516958836</v>
+        <v>74.4939673277577</v>
       </c>
       <c r="H38" t="n">
-        <v>27.86700541216357</v>
+        <v>356.312828375576</v>
       </c>
       <c r="I38" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J38" t="n">
-        <v>15.465290491431375</v>
+        <v>100.50200976380124</v>
       </c>
       <c r="K38" t="n">
-        <v>326.72069076444615</v>
+        <v>2708.5809558041733</v>
       </c>
       <c r="L38" t="n">
-        <v>59.107029770305246</v>
+        <v>603.895793016975</v>
       </c>
       <c r="M38" t="n">
-        <v>29.36775997729088</v>
+        <v>202.7677542520418</v>
       </c>
       <c r="N38" t="n">
-        <v>683.0249695439726</v>
+        <v>2780.6461354776684</v>
       </c>
       <c r="O38" t="n">
-        <v>647.2933528594825</v>
+        <v>5037.535685479224</v>
       </c>
       <c r="P38" t="n">
-        <v>127.15720918360985</v>
+        <v>671.8897705561623</v>
       </c>
       <c r="Q38" t="n">
-        <v>554.6926764456123</v>
+        <v>2833.791872132946</v>
       </c>
       <c r="R38" t="n">
-        <v>373.6539228578489</v>
+        <v>1181.174668111491</v>
       </c>
       <c r="S38" t="n">
-        <v>805.1724237454057</v>
+        <v>7349.080815703511</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E39" t="n">
-        <v>908.5144758820953</v>
+        <v>89.39994231252723</v>
       </c>
       <c r="F39" t="n">
-        <v>4097.97001043291</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G39" t="n">
-        <v>70.6017789871674</v>
+        <v>10.775372516958836</v>
       </c>
       <c r="H39" t="n">
-        <v>378.84068488103253</v>
+        <v>27.86700541216357</v>
       </c>
       <c r="I39" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J39" t="n">
-        <v>109.61569851908737</v>
+        <v>15.465290491431375</v>
       </c>
       <c r="K39" t="n">
-        <v>2557.8103623343172</v>
+        <v>326.72069076444615</v>
       </c>
       <c r="L39" t="n">
-        <v>560.9195622634386</v>
+        <v>59.107029770305246</v>
       </c>
       <c r="M39" t="n">
-        <v>198.62890922752075</v>
+        <v>29.36775997729088</v>
       </c>
       <c r="N39" t="n">
-        <v>4394.59673541186</v>
+        <v>683.0249695439726</v>
       </c>
       <c r="O39" t="n">
-        <v>6622.068528506834</v>
+        <v>647.2933528594825</v>
       </c>
       <c r="P39" t="n">
-        <v>926.7457709716515</v>
+        <v>127.15720918360985</v>
       </c>
       <c r="Q39" t="n">
-        <v>4320.606778867492</v>
+        <v>554.6926764456123</v>
       </c>
       <c r="R39" t="n">
-        <v>2010.7812513134093</v>
+        <v>373.6539228578489</v>
       </c>
       <c r="S39" t="n">
-        <v>6359.880571405437</v>
+        <v>805.1724237454057</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E40" t="n">
-        <v>293.3972876686744</v>
+        <v>908.5144758820953</v>
       </c>
       <c r="F40" t="n">
-        <v>4425.918303739955</v>
+        <v>4097.97001043291</v>
       </c>
       <c r="G40" t="n">
-        <v>31.65170234175463</v>
+        <v>70.6017789871674</v>
       </c>
       <c r="H40" t="n">
-        <v>143.78554775733494</v>
+        <v>378.84068488103253</v>
       </c>
       <c r="I40" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J40" t="n">
-        <v>39.92150631845578</v>
+        <v>109.61569851908737</v>
       </c>
       <c r="K40" t="n">
-        <v>1000.4281906734404</v>
+        <v>2557.8103623343172</v>
       </c>
       <c r="L40" t="n">
-        <v>213.02089030763042</v>
+        <v>560.9195622634386</v>
       </c>
       <c r="M40" t="n">
-        <v>76.90504070797657</v>
+        <v>198.62890922752075</v>
       </c>
       <c r="N40" t="n">
-        <v>1148.29431751482</v>
+        <v>4394.59673541186</v>
       </c>
       <c r="O40" t="n">
-        <v>1867.6945130858467</v>
+        <v>6622.068528506834</v>
       </c>
       <c r="P40" t="n">
-        <v>282.61615961563865</v>
+        <v>926.7457709716515</v>
       </c>
       <c r="Q40" t="n">
-        <v>1505.1320293926653</v>
+        <v>4320.606778867492</v>
       </c>
       <c r="R40" t="n">
-        <v>608.5728389874603</v>
+        <v>2010.7812513134093</v>
       </c>
       <c r="S40" t="n">
-        <v>2120.7469971754654</v>
+        <v>6359.880571405437</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E41" t="n">
-        <v>636.304441705207</v>
+        <v>293.3972876686744</v>
       </c>
       <c r="F41" t="n">
-        <v>5258.200586454538</v>
+        <v>4425.918303739955</v>
       </c>
       <c r="G41" t="n">
-        <v>61.53336265423614</v>
+        <v>31.65170234175463</v>
       </c>
       <c r="H41" t="n">
-        <v>294.2968572853134</v>
+        <v>143.78554775733494</v>
       </c>
       <c r="I41" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J41" t="n">
-        <v>71.14296069082603</v>
+        <v>39.92150631845578</v>
       </c>
       <c r="K41" t="n">
-        <v>1824.2953749325582</v>
+        <v>1000.4281906734404</v>
       </c>
       <c r="L41" t="n">
-        <v>408.81977414580274</v>
+        <v>213.02089030763042</v>
       </c>
       <c r="M41" t="n">
-        <v>154.48207627990587</v>
+        <v>76.90504070797657</v>
       </c>
       <c r="N41" t="n">
-        <v>4391.711883079517</v>
+        <v>1148.29431751482</v>
       </c>
       <c r="O41" t="n">
-        <v>9630.387474517283</v>
+        <v>1867.6945130858467</v>
       </c>
       <c r="P41" t="n">
-        <v>1021.5586663073564</v>
+        <v>282.61615961563865</v>
       </c>
       <c r="Q41" t="n">
-        <v>5632.334478916302</v>
+        <v>1505.1320293926653</v>
       </c>
       <c r="R41" t="n">
-        <v>5120.670408175457</v>
+        <v>608.5728389874603</v>
       </c>
       <c r="S41" t="n">
-        <v>17468.67413578378</v>
+        <v>2120.7469971754654</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E42" t="n">
-        <v>768.6757794177962</v>
+        <v>636.304441705207</v>
       </c>
       <c r="F42" t="n">
-        <v>5332.433289178851</v>
+        <v>5258.200586454538</v>
       </c>
       <c r="G42" t="n">
-        <v>76.26918512424004</v>
+        <v>61.53336265423614</v>
       </c>
       <c r="H42" t="n">
-        <v>258.3338664504567</v>
+        <v>294.2968572853134</v>
       </c>
       <c r="I42" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J42" t="n">
-        <v>77.12299958808993</v>
+        <v>71.14296069082603</v>
       </c>
       <c r="K42" t="n">
-        <v>1122.7176730069414</v>
+        <v>1824.2953749325582</v>
       </c>
       <c r="L42" t="n">
-        <v>240.97393002471313</v>
+        <v>408.81977414580274</v>
       </c>
       <c r="M42" t="n">
-        <v>92.65670331744194</v>
+        <v>154.48207627990587</v>
       </c>
       <c r="N42" t="n">
-        <v>11897.992879381456</v>
+        <v>4391.711883079517</v>
       </c>
       <c r="O42" t="n">
-        <v>2780.3384713852965</v>
+        <v>9630.387474517283</v>
       </c>
       <c r="P42" t="n">
-        <v>1649.6385014879454</v>
+        <v>1021.5586663073564</v>
       </c>
       <c r="Q42" t="n">
-        <v>1761.7222663011976</v>
+        <v>5632.334478916302</v>
       </c>
       <c r="R42" t="n">
-        <v>5393.331635580115</v>
+        <v>5120.670408175457</v>
       </c>
       <c r="S42" t="n">
-        <v>2408.5379502429423</v>
+        <v>17468.67413578378</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E43" t="n">
-        <v>1336.215142285475</v>
+        <v>768.6757794177962</v>
       </c>
       <c r="F43" t="n">
-        <v>21092.113875615374</v>
+        <v>5332.433289178851</v>
       </c>
       <c r="G43" t="n">
-        <v>128.89882412756216</v>
+        <v>76.26918512424004</v>
       </c>
       <c r="H43" t="n">
-        <v>539.0421162835638</v>
+        <v>258.3338664504567</v>
       </c>
       <c r="I43" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J43" t="n">
-        <v>159.41600067599038</v>
+        <v>77.12299958808993</v>
       </c>
       <c r="K43" t="n">
-        <v>3358.933176718943</v>
+        <v>1122.7176730069414</v>
       </c>
       <c r="L43" t="n">
-        <v>749.6642322285538</v>
+        <v>240.97393002471313</v>
       </c>
       <c r="M43" t="n">
-        <v>269.5688687991397</v>
+        <v>92.65670331744194</v>
       </c>
       <c r="N43" t="n">
-        <v>10822.99412615197</v>
+        <v>11897.992879381456</v>
       </c>
       <c r="O43" t="n">
-        <v>24314.22613528814</v>
+        <v>2780.3384713852965</v>
       </c>
       <c r="P43" t="n">
-        <v>2988.425451183327</v>
+        <v>1649.6385014879454</v>
       </c>
       <c r="Q43" t="n">
-        <v>15061.734034856925</v>
+        <v>1761.7222663011976</v>
       </c>
       <c r="R43" t="n">
-        <v>6200.094692713447</v>
+        <v>5393.331635580115</v>
       </c>
       <c r="S43" t="n">
-        <v>22736.68760565857</v>
+        <v>2408.5379502429423</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E44" t="n">
-        <v>1208.6907989038757</v>
+        <v>1336.215142285475</v>
       </c>
       <c r="F44" t="n">
-        <v>4641.436122323263</v>
+        <v>21092.113875615374</v>
       </c>
       <c r="G44" t="n">
-        <v>112.69236857931095</v>
+        <v>128.89882412756216</v>
       </c>
       <c r="H44" t="n">
-        <v>456.42820666245365</v>
+        <v>539.0421162835638</v>
       </c>
       <c r="I44" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J44" t="n">
-        <v>155.67577413190813</v>
+        <v>159.41600067599038</v>
       </c>
       <c r="K44" t="n">
-        <v>1150.9732375390258</v>
+        <v>3358.933176718943</v>
       </c>
       <c r="L44" t="n">
-        <v>275.57695761406563</v>
+        <v>749.6642322285538</v>
       </c>
       <c r="M44" t="n">
-        <v>94.61820692864045</v>
+        <v>269.5688687991397</v>
       </c>
       <c r="N44" t="n">
-        <v>1220.8339929425365</v>
+        <v>10822.99412615197</v>
       </c>
       <c r="O44" t="n">
-        <v>2228.6947990723847</v>
+        <v>24314.22613528814</v>
       </c>
       <c r="P44" t="n">
-        <v>322.7447695160237</v>
+        <v>2988.425451183327</v>
       </c>
       <c r="Q44" t="n">
-        <v>1733.7456229434017</v>
+        <v>15061.734034856925</v>
       </c>
       <c r="R44" t="n">
-        <v>661.1497252993405</v>
+        <v>6200.094692713447</v>
       </c>
       <c r="S44" t="n">
-        <v>2646.389486539533</v>
+        <v>22736.68760565857</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E45" t="n">
-        <v>25701.981356148965</v>
+        <v>1208.6907989038757</v>
       </c>
       <c r="F45" t="n">
-        <v>13427.033909830472</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G45" t="n">
-        <v>2316.183125677189</v>
+        <v>112.69236857931095</v>
       </c>
       <c r="H45" t="n">
-        <v>10557.72288868422</v>
+        <v>456.42820666245365</v>
       </c>
       <c r="I45" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J45" t="n">
-        <v>2939.378040974826</v>
+        <v>155.67577413190813</v>
       </c>
       <c r="K45" t="n">
-        <v>49349.22327149315</v>
+        <v>1150.9732375390258</v>
       </c>
       <c r="L45" t="n">
-        <v>10451.567133231702</v>
+        <v>275.57695761406563</v>
       </c>
       <c r="M45" t="n">
-        <v>3932.484652640725</v>
+        <v>94.61820692864045</v>
       </c>
       <c r="N45" t="n">
-        <v>95788.80233883348</v>
+        <v>1220.8339929425365</v>
       </c>
       <c r="O45" t="n">
-        <v>106322.95157664194</v>
+        <v>2228.6947990723847</v>
       </c>
       <c r="P45" t="n">
-        <v>22612.556483760873</v>
+        <v>322.7447695160237</v>
       </c>
       <c r="Q45" t="n">
-        <v>73079.83455227377</v>
+        <v>1733.7456229434017</v>
       </c>
       <c r="R45" t="n">
-        <v>42475.30126586585</v>
+        <v>661.1497252993405</v>
       </c>
       <c r="S45" t="n">
-        <v>109050.389015109</v>
+        <v>2646.389486539533</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B46" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E46" t="n">
-        <v>327.0181022155551</v>
+        <v>25701.981356148965</v>
       </c>
       <c r="F46" t="n">
-        <v>4641.436122323263</v>
+        <v>13427.033909830472</v>
       </c>
       <c r="G46" t="n">
-        <v>27.269401401605222</v>
+        <v>2316.183125677189</v>
       </c>
       <c r="H46" t="n">
-        <v>126.8625411023056</v>
+        <v>10557.72288868422</v>
       </c>
       <c r="I46" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J46" t="n">
-        <v>40.877726885199415</v>
+        <v>2939.378040974826</v>
       </c>
       <c r="K46" t="n">
-        <v>9423.04165071321</v>
+        <v>49349.22327149315</v>
       </c>
       <c r="L46" t="n">
-        <v>2157.041181393869</v>
+        <v>10451.567133231702</v>
       </c>
       <c r="M46" t="n">
-        <v>758.8778746248709</v>
+        <v>3932.484652640725</v>
       </c>
       <c r="N46" t="n">
-        <v>1824.724596113616</v>
+        <v>95788.80233883348</v>
       </c>
       <c r="O46" t="n">
-        <v>4356.961134639303</v>
+        <v>106322.95157664194</v>
       </c>
       <c r="P46" t="n">
-        <v>487.8138397311315</v>
+        <v>22612.556483760873</v>
       </c>
       <c r="Q46" t="n">
-        <v>3479.9477951247077</v>
+        <v>73079.83455227377</v>
       </c>
       <c r="R46" t="n">
-        <v>1368.5004501687185</v>
+        <v>42475.30126586585</v>
       </c>
       <c r="S46" t="n">
-        <v>10649.064364393946</v>
+        <v>109050.389015109</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>75</v>
       </c>
       <c r="E47" t="n">
-        <v>384.54278774434147</v>
+        <v>327.0181022155551</v>
       </c>
       <c r="F47" t="n">
-        <v>8784.151029746843</v>
+        <v>4641.436122323263</v>
       </c>
       <c r="G47" t="n">
-        <v>57.1085046676534</v>
+        <v>27.269401401605222</v>
       </c>
       <c r="H47" t="n">
-        <v>126.16454399097526</v>
+        <v>126.8625411023056</v>
       </c>
       <c r="I47" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J47" t="n">
-        <v>50.54486619771224</v>
+        <v>40.877726885199415</v>
       </c>
       <c r="K47" t="n">
-        <v>1318.4388993873808</v>
+        <v>9423.04165071321</v>
       </c>
       <c r="L47" t="n">
-        <v>224.3051134025214</v>
+        <v>2157.041181393869</v>
       </c>
       <c r="M47" t="n">
-        <v>92.88580561499208</v>
+        <v>758.8778746248709</v>
       </c>
       <c r="N47" t="n">
-        <v>1244.2570792163317</v>
+        <v>1824.724596113616</v>
       </c>
       <c r="O47" t="n">
-        <v>2410.328204620374</v>
+        <v>4356.961134639303</v>
       </c>
       <c r="P47" t="n">
-        <v>388.80101875252154</v>
+        <v>487.8138397311315</v>
       </c>
       <c r="Q47" t="n">
-        <v>2258.788969461873</v>
+        <v>3479.9477951247077</v>
       </c>
       <c r="R47" t="n">
-        <v>725.3752229567119</v>
+        <v>1368.5004501687185</v>
       </c>
       <c r="S47" t="n">
-        <v>2663.1822958799385</v>
+        <v>10649.064364393946</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E48" t="n">
-        <v>3910.9142174750395</v>
+        <v>384.54278774434147</v>
       </c>
       <c r="F48" t="n">
-        <v>10603.848260735405</v>
+        <v>8784.151029746843</v>
       </c>
       <c r="G48" t="n">
-        <v>396.3988114611008</v>
+        <v>57.1085046676534</v>
       </c>
       <c r="H48" t="n">
-        <v>1604.5934578702484</v>
+        <v>126.16454399097526</v>
       </c>
       <c r="I48" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J48" t="n">
-        <v>499.66814827505107</v>
+        <v>50.54486619771224</v>
       </c>
       <c r="K48" t="n">
-        <v>24661.152080360233</v>
+        <v>1318.4388993873808</v>
       </c>
       <c r="L48" t="n">
-        <v>5127.337576895256</v>
+        <v>224.3051134025214</v>
       </c>
       <c r="M48" t="n">
-        <v>1921.3239490773904</v>
+        <v>92.88580561499208</v>
       </c>
       <c r="N48" t="n">
-        <v>77248.78953444907</v>
+        <v>1244.2570792163317</v>
       </c>
       <c r="O48" t="n">
-        <v>95727.83367274822</v>
+        <v>2410.328204620374</v>
       </c>
       <c r="P48" t="n">
-        <v>16195.490775169656</v>
+        <v>388.80101875252154</v>
       </c>
       <c r="Q48" t="n">
-        <v>72701.71332332848</v>
+        <v>2258.788969461873</v>
       </c>
       <c r="R48" t="n">
-        <v>43303.016279153686</v>
+        <v>725.3752229567119</v>
       </c>
       <c r="S48" t="n">
-        <v>122070.89948516102</v>
+        <v>2663.1822958799385</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="E49" t="n">
-        <v>1154.9262620992208</v>
+        <v>3910.9142174750395</v>
       </c>
       <c r="F49" t="n">
-        <v>4641.436122323263</v>
+        <v>10603.848260735405</v>
       </c>
       <c r="G49" t="n">
-        <v>136.9137028829668</v>
+        <v>396.3988114611008</v>
       </c>
       <c r="H49" t="n">
-        <v>581.6746085392293</v>
+        <v>1604.5934578702484</v>
       </c>
       <c r="I49" t="n">
         <v>4079.717242512663</v>
       </c>
       <c r="J49" t="n">
+        <v>499.66814827505107</v>
+      </c>
+      <c r="K49" t="n">
+        <v>24661.152080360233</v>
+      </c>
+      <c r="L49" t="n">
+        <v>5127.337576895256</v>
+      </c>
+      <c r="M49" t="n">
+        <v>1921.3239490773904</v>
+      </c>
+      <c r="N49" t="n">
+        <v>77248.78953444907</v>
+      </c>
+      <c r="O49" t="n">
+        <v>95727.83367274822</v>
+      </c>
+      <c r="P49" t="n">
+        <v>16195.490775169656</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>72701.71332332848</v>
+      </c>
+      <c r="R49" t="n">
+        <v>43303.016279153686</v>
+      </c>
+      <c r="S49" t="n">
+        <v>122070.89948516102</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1154.9262620992208</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4641.436122323263</v>
+      </c>
+      <c r="G50" t="n">
+        <v>136.9137028829668</v>
+      </c>
+      <c r="H50" t="n">
+        <v>581.6746085392293</v>
+      </c>
+      <c r="I50" t="n">
+        <v>4079.717242512663</v>
+      </c>
+      <c r="J50" t="n">
         <v>192.09583578590366</v>
       </c>
-      <c r="K49" t="n">
+      <c r="K50" t="n">
         <v>2422.4718496875466</v>
       </c>
-      <c r="L49" t="n">
+      <c r="L50" t="n">
         <v>523.4676286390147</v>
       </c>
-      <c r="M49" t="n">
+      <c r="M50" t="n">
         <v>188.8906958229306</v>
       </c>
-      <c r="N49" t="n">
+      <c r="N50" t="n">
         <v>21705.59796635315</v>
       </c>
-      <c r="O49" t="n">
+      <c r="O50" t="n">
         <v>39742.73768486481</v>
       </c>
-      <c r="P49" t="n">
+      <c r="P50" t="n">
         <v>5445.036085408454</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="Q50" t="n">
         <v>25495.591507779776</v>
       </c>
-      <c r="R49" t="n">
+      <c r="R50" t="n">
         <v>7268.925403578192</v>
       </c>
-      <c r="S49" t="n">
+      <c r="S50" t="n">
         <v>24547.902016859203</v>
       </c>
     </row>

</xml_diff>